<commit_message>
update bert imdb results
</commit_message>
<xml_diff>
--- a/noise_attack_results/IMDB_0.1_scale_clean_accuracy_results.xlsx
+++ b/noise_attack_results/IMDB_0.1_scale_clean_accuracy_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
   <si>
     <t>noise_type\intensity</t>
   </si>
@@ -25,118 +25,172 @@
     <t>0.1</t>
   </si>
   <si>
-    <t>92.91%</t>
+    <t>91.88%</t>
   </si>
   <si>
     <t>0.2</t>
   </si>
   <si>
-    <t>91.70%</t>
+    <t>91.00%</t>
   </si>
   <si>
     <t>0.3</t>
   </si>
   <si>
-    <t>84.60%</t>
+    <t>86.62%</t>
   </si>
   <si>
     <t>0.4</t>
   </si>
   <si>
-    <t>63.48%</t>
+    <t>64.70%</t>
   </si>
   <si>
     <t>0.5</t>
   </si>
   <si>
-    <t>53.45%</t>
+    <t>54.00%</t>
   </si>
   <si>
     <t>0.6</t>
   </si>
   <si>
-    <t>51.03%</t>
+    <t>51.21%</t>
   </si>
   <si>
     <t>0.7</t>
   </si>
   <si>
-    <t>50.71%</t>
+    <t>50.62%</t>
   </si>
   <si>
     <t>0.8</t>
   </si>
   <si>
-    <t>50.35%</t>
+    <t>50.16%</t>
   </si>
   <si>
     <t>0.9</t>
   </si>
   <si>
-    <t>50.26%</t>
+    <t>50.06%</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>50.01%</t>
+    <t>50.07%</t>
+  </si>
+  <si>
+    <t>pre_att_cls</t>
+  </si>
+  <si>
+    <t>92.10%</t>
+  </si>
+  <si>
+    <t>91.96%</t>
+  </si>
+  <si>
+    <t>91.76%</t>
+  </si>
+  <si>
+    <t>90.88%</t>
+  </si>
+  <si>
+    <t>89.49%</t>
+  </si>
+  <si>
+    <t>88.06%</t>
+  </si>
+  <si>
+    <t>86.26%</t>
+  </si>
+  <si>
+    <t>84.26%</t>
+  </si>
+  <si>
+    <t>81.83%</t>
   </si>
   <si>
     <t>post_att_all</t>
   </si>
   <si>
-    <t>93.01%</t>
-  </si>
-  <si>
-    <t>92.71%</t>
-  </si>
-  <si>
-    <t>91.14%</t>
-  </si>
-  <si>
-    <t>83.38%</t>
-  </si>
-  <si>
-    <t>68.63%</t>
-  </si>
-  <si>
-    <t>60.69%</t>
-  </si>
-  <si>
-    <t>52.85%</t>
-  </si>
-  <si>
-    <t>50.37%</t>
-  </si>
-  <si>
-    <t>50.15%</t>
-  </si>
-  <si>
-    <t>50.13%</t>
+    <t>92.05%</t>
+  </si>
+  <si>
+    <t>91.73%</t>
+  </si>
+  <si>
+    <t>90.81%</t>
+  </si>
+  <si>
+    <t>86.95%</t>
+  </si>
+  <si>
+    <t>74.22%</t>
+  </si>
+  <si>
+    <t>58.20%</t>
+  </si>
+  <si>
+    <t>52.30%</t>
+  </si>
+  <si>
+    <t>50.76%</t>
+  </si>
+  <si>
+    <t>50.02%</t>
+  </si>
+  <si>
+    <t>post_att_cls</t>
+  </si>
+  <si>
+    <t>92.11%</t>
+  </si>
+  <si>
+    <t>92.03%</t>
+  </si>
+  <si>
+    <t>91.93%</t>
+  </si>
+  <si>
+    <t>91.87%</t>
+  </si>
+  <si>
+    <t>91.17%</t>
+  </si>
+  <si>
+    <t>89.64%</t>
+  </si>
+  <si>
+    <t>87.49%</t>
+  </si>
+  <si>
+    <t>84.96%</t>
   </si>
   <si>
     <t>last_cls</t>
   </si>
   <si>
-    <t>93.04%</t>
-  </si>
-  <si>
-    <t>93.02%</t>
-  </si>
-  <si>
-    <t>93.03%</t>
-  </si>
-  <si>
-    <t>93.05%</t>
-  </si>
-  <si>
-    <t>93.06%</t>
+    <t>92.14%</t>
+  </si>
+  <si>
+    <t>92.15%</t>
+  </si>
+  <si>
+    <t>92.16%</t>
+  </si>
+  <si>
+    <t>92.12%</t>
+  </si>
+  <si>
+    <t>92.13%</t>
   </si>
   <si>
     <t>logits</t>
   </si>
   <si>
-    <t>92.99%</t>
+    <t>92.09%</t>
   </si>
 </sst>
 </file>
@@ -471,7 +525,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -559,101 +613,171 @@
         <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>